<commit_message>
Add files to website
</commit_message>
<xml_diff>
--- a/data/finance-minister.xlsx
+++ b/data/finance-minister.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\RepTemplates\data_analytics\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{139F287F-5F95-4CC0-8099-16D5B1DD8DDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C9A749F-ABAC-406F-9FB4-024461B2ECD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CADBB125-9199-438F-B766-4237F94889CD}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{CADBB125-9199-438F-B766-4237F94889CD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1 (4)" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="46">
   <si>
     <t>Miftah Ismail, Ishaq Dar</t>
   </si>
@@ -141,28 +142,40 @@
     <t>policy</t>
   </si>
   <si>
-    <t>time</t>
-  </si>
-  <si>
-    <t>education</t>
-  </si>
-  <si>
-    <t>1990-1992</t>
-  </si>
-  <si>
-    <t>Master</t>
-  </si>
-  <si>
-    <t>size</t>
-  </si>
-  <si>
-    <t>2002-2007</t>
-  </si>
-  <si>
-    <t>PhD</t>
-  </si>
-  <si>
     <t>US dominated agenda by PTI</t>
+  </si>
+  <si>
+    <t>Prime Minister</t>
+  </si>
+  <si>
+    <t xml:space="preserve">start_date </t>
+  </si>
+  <si>
+    <t>end_date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Husyen Shaheed Suharwardy </t>
+  </si>
+  <si>
+    <t>Zulfikar Ali Bhutto</t>
+  </si>
+  <si>
+    <t>Benazir Bhutto</t>
+  </si>
+  <si>
+    <t>Nawaz Sharif</t>
+  </si>
+  <si>
+    <t>Shahid Khaqan Abbasi</t>
+  </si>
+  <si>
+    <t>Yousaf Raza Gillani</t>
+  </si>
+  <si>
+    <t>Shehbaz Saharif</t>
+  </si>
+  <si>
+    <t>Imran Khan</t>
   </si>
 </sst>
 </file>
@@ -538,7 +551,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27AECC1A-6815-439E-AA07-E0CC88E6B93B}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B6" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView topLeftCell="B6" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
@@ -743,7 +756,7 @@
         <v>2</v>
       </c>
       <c r="F10" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -773,48 +786,140 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CE8FCBA-261E-4F63-A42F-78D35E7A6F99}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="3" width="10.5546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B2">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>37</v>
+        <v>38</v>
+      </c>
+      <c r="B2" s="1">
+        <v>22647</v>
+      </c>
+      <c r="C2" s="1">
+        <v>23012</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>39</v>
       </c>
-      <c r="B3">
-        <v>-5</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="B3" s="1">
+        <v>28369</v>
+      </c>
+      <c r="C3" s="1">
+        <v>28949</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>40</v>
+      </c>
+      <c r="B4" s="1">
+        <v>31625</v>
+      </c>
+      <c r="C4" s="1">
+        <v>31717</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" s="1">
+        <v>35166</v>
+      </c>
+      <c r="C5" s="1">
+        <v>35394</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" s="1">
+        <v>36452</v>
+      </c>
+      <c r="C6" s="1">
+        <v>36445</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7" s="1">
+        <v>43294</v>
+      </c>
+      <c r="C7" s="1">
+        <v>43796</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" s="1">
+        <v>43664</v>
+      </c>
+      <c r="C8" s="1">
+        <v>43918</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9" s="1">
+        <v>43595</v>
+      </c>
+      <c r="C9" s="1">
+        <v>43614</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" s="1">
+        <v>44308</v>
+      </c>
+      <c r="C10" s="1">
+        <v>44832</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11" s="1">
+        <v>45174</v>
+      </c>
+      <c r="C11" s="1">
+        <v>45265</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>